<commit_message>
New test results added
</commit_message>
<xml_diff>
--- a/27.xlsx
+++ b/27.xlsx
@@ -1,15 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="20225"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\bfarleigh1\Desktop\FPix2\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="16080" yWindow="0" windowWidth="15060" windowHeight="20520" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="16060" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -17,7 +12,7 @@
   <definedNames>
     <definedName name="_xlnm.Print_Area" localSheetId="0">Sheet1!$A$1:$N$80</definedName>
   </definedNames>
-  <calcPr calcId="152511" concurrentCalc="0"/>
+  <calcPr calcId="140001" concurrentCalc="0"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
@@ -27,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="278" uniqueCount="99">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="280" uniqueCount="101">
   <si>
     <t>Test all connections listed in the table below and record the values observed. Use the test points on the adapter board.</t>
   </si>
@@ -230,9 +225,6 @@
     <t>Final decision:</t>
   </si>
   <si>
-    <t>n</t>
-  </si>
-  <si>
     <t>1) Do not connect the adapter. Turn HV on, read after 60 sec</t>
   </si>
   <si>
@@ -324,6 +316,15 @@
   </si>
   <si>
     <t>Corrected</t>
+  </si>
+  <si>
+    <t>y</t>
+  </si>
+  <si>
+    <t>pass</t>
+  </si>
+  <si>
+    <t>Amanda</t>
   </si>
 </sst>
 </file>
@@ -1238,106 +1239,106 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <sheetPr>
+  <sheetPr enableFormatConditionsCalculation="0">
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
   <dimension ref="A1:P80"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A17" workbookViewId="0">
-      <selection activeCell="H53" sqref="H53"/>
+    <sheetView tabSelected="1" topLeftCell="A50" workbookViewId="0">
+      <selection activeCell="B81" sqref="B81"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <cols>
     <col min="1" max="1" width="12.5" customWidth="1"/>
-    <col min="3" max="3" width="8.375" style="5" customWidth="1"/>
-    <col min="4" max="4" width="13.125" style="5" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="10.875" style="9"/>
-    <col min="6" max="6" width="10.875" style="5"/>
-    <col min="9" max="9" width="5.875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="8.33203125" style="5" customWidth="1"/>
+    <col min="4" max="4" width="13.1640625" style="5" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="11" style="9"/>
+    <col min="6" max="6" width="11.33203125" style="5" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="5.83203125" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="6.5" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="12" style="9" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="4.875" style="9" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="4.83203125" style="9" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" ht="26.25" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:15" ht="26.25">
       <c r="A1" s="2" t="s">
-        <v>91</v>
-      </c>
-    </row>
-    <row r="3" spans="1:15" ht="18.75" x14ac:dyDescent="0.3">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="3" spans="1:15" ht="18.75">
       <c r="A3" s="1" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="B3" s="28"/>
       <c r="C3" s="32">
         <v>27</v>
       </c>
     </row>
-    <row r="4" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:15">
       <c r="B4" s="28"/>
     </row>
-    <row r="5" spans="1:15" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:15" ht="18.75">
       <c r="A5" s="1" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="B5" s="28"/>
       <c r="C5" s="29" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="D5" s="9" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="6" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:15">
       <c r="A6" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="B6" s="28"/>
       <c r="C6" s="30" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="D6" s="31">
         <v>79980109</v>
       </c>
       <c r="F6" s="17" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="H6" s="27"/>
       <c r="I6" t="s">
         <v>51</v>
       </c>
     </row>
-    <row r="7" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:15">
       <c r="A7" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="B7" s="28"/>
       <c r="C7" s="30" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="D7" s="31"/>
     </row>
-    <row r="8" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:15">
       <c r="A8" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="B8" s="28"/>
       <c r="C8" s="30" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="D8" s="31"/>
     </row>
-    <row r="9" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:15">
       <c r="B9" s="28"/>
       <c r="C9" s="21"/>
     </row>
-    <row r="11" spans="1:15" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:15" ht="18.75">
       <c r="A11" s="1" t="s">
         <v>53</v>
       </c>
     </row>
-    <row r="13" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:15">
       <c r="A13" t="s">
         <v>1</v>
       </c>
@@ -1345,7 +1346,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="14" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:15">
       <c r="A14" t="s">
         <v>3</v>
       </c>
@@ -1353,17 +1354,17 @@
         <v>0</v>
       </c>
     </row>
-    <row r="15" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:15">
       <c r="B15" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="16" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:15">
       <c r="O16" s="18" t="s">
         <v>65</v>
       </c>
     </row>
-    <row r="17" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:16">
       <c r="A17" s="3" t="s">
         <v>4</v>
       </c>
@@ -1401,7 +1402,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="18" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:16">
       <c r="A18" t="s">
         <v>8</v>
       </c>
@@ -1430,10 +1431,12 @@
       <c r="J18" t="s">
         <v>13</v>
       </c>
-      <c r="K18" s="12"/>
+      <c r="K18" s="12">
+        <v>0.7</v>
+      </c>
       <c r="L18" s="9" t="str">
         <f t="shared" ref="L18:L33" si="0">IF(AND(K18&lt;K$34,ISNUMBER(K18)),"ok","NOK")</f>
-        <v>NOK</v>
+        <v>ok</v>
       </c>
       <c r="O18">
         <f t="shared" ref="O18:O51" si="1">IF(G18="NOK",1,0)</f>
@@ -1441,10 +1444,10 @@
       </c>
       <c r="P18">
         <f>IF(L18="NOK",1,0)</f>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="19" spans="1:16" x14ac:dyDescent="0.25">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="19" spans="1:16">
       <c r="A19" t="s">
         <v>8</v>
       </c>
@@ -1473,10 +1476,12 @@
       <c r="J19" t="s">
         <v>14</v>
       </c>
-      <c r="K19" s="12"/>
+      <c r="K19" s="12">
+        <v>0.7</v>
+      </c>
       <c r="L19" s="9" t="str">
         <f t="shared" si="0"/>
-        <v>NOK</v>
+        <v>ok</v>
       </c>
       <c r="O19">
         <f t="shared" si="1"/>
@@ -1484,10 +1489,10 @@
       </c>
       <c r="P19">
         <f t="shared" ref="P19:P33" si="2">IF(L19="NOK",1,0)</f>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="20" spans="1:16" x14ac:dyDescent="0.25">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="20" spans="1:16">
       <c r="A20" t="s">
         <v>8</v>
       </c>
@@ -1517,10 +1522,12 @@
       <c r="J20" t="s">
         <v>9</v>
       </c>
-      <c r="K20" s="12"/>
+      <c r="K20" s="12">
+        <v>0.7</v>
+      </c>
       <c r="L20" s="9" t="str">
         <f t="shared" si="0"/>
-        <v>NOK</v>
+        <v>ok</v>
       </c>
       <c r="O20">
         <f t="shared" si="1"/>
@@ -1528,10 +1535,10 @@
       </c>
       <c r="P20">
         <f t="shared" si="2"/>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="21" spans="1:16" x14ac:dyDescent="0.25">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="21" spans="1:16">
       <c r="A21" t="s">
         <v>8</v>
       </c>
@@ -1561,10 +1568,12 @@
       <c r="J21" t="s">
         <v>9</v>
       </c>
-      <c r="K21" s="12"/>
+      <c r="K21" s="12">
+        <v>0.7</v>
+      </c>
       <c r="L21" s="9" t="str">
         <f t="shared" si="0"/>
-        <v>NOK</v>
+        <v>ok</v>
       </c>
       <c r="O21">
         <f t="shared" si="1"/>
@@ -1572,10 +1581,10 @@
       </c>
       <c r="P21">
         <f t="shared" si="2"/>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="22" spans="1:16" x14ac:dyDescent="0.25">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="22" spans="1:16">
       <c r="A22" t="s">
         <v>8</v>
       </c>
@@ -1604,10 +1613,12 @@
       <c r="J22" t="s">
         <v>15</v>
       </c>
-      <c r="K22" s="12"/>
+      <c r="K22" s="12">
+        <v>0.7</v>
+      </c>
       <c r="L22" s="9" t="str">
         <f t="shared" si="0"/>
-        <v>NOK</v>
+        <v>ok</v>
       </c>
       <c r="O22">
         <f t="shared" si="1"/>
@@ -1615,10 +1626,10 @@
       </c>
       <c r="P22">
         <f t="shared" si="2"/>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="23" spans="1:16" x14ac:dyDescent="0.25">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="23" spans="1:16">
       <c r="A23" t="s">
         <v>8</v>
       </c>
@@ -1647,10 +1658,12 @@
       <c r="J23" t="s">
         <v>16</v>
       </c>
-      <c r="K23" s="12"/>
+      <c r="K23" s="12">
+        <v>0.7</v>
+      </c>
       <c r="L23" s="9" t="str">
         <f t="shared" si="0"/>
-        <v>NOK</v>
+        <v>ok</v>
       </c>
       <c r="O23">
         <f t="shared" si="1"/>
@@ -1658,10 +1671,10 @@
       </c>
       <c r="P23">
         <f t="shared" si="2"/>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="24" spans="1:16" x14ac:dyDescent="0.25">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="24" spans="1:16">
       <c r="A24" t="s">
         <v>8</v>
       </c>
@@ -1690,10 +1703,12 @@
       <c r="J24" t="s">
         <v>17</v>
       </c>
-      <c r="K24" s="12"/>
+      <c r="K24" s="12">
+        <v>0.7</v>
+      </c>
       <c r="L24" s="9" t="str">
         <f t="shared" si="0"/>
-        <v>NOK</v>
+        <v>ok</v>
       </c>
       <c r="O24">
         <f t="shared" si="1"/>
@@ -1701,10 +1716,10 @@
       </c>
       <c r="P24">
         <f t="shared" si="2"/>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="25" spans="1:16" x14ac:dyDescent="0.25">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="25" spans="1:16">
       <c r="A25" t="s">
         <v>8</v>
       </c>
@@ -1733,10 +1748,12 @@
       <c r="J25" t="s">
         <v>18</v>
       </c>
-      <c r="K25" s="12"/>
+      <c r="K25" s="12">
+        <v>0.7</v>
+      </c>
       <c r="L25" s="9" t="str">
         <f t="shared" si="0"/>
-        <v>NOK</v>
+        <v>ok</v>
       </c>
       <c r="O25">
         <f t="shared" si="1"/>
@@ -1744,10 +1761,10 @@
       </c>
       <c r="P25">
         <f t="shared" si="2"/>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="26" spans="1:16" x14ac:dyDescent="0.25">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="26" spans="1:16">
       <c r="A26" t="s">
         <v>8</v>
       </c>
@@ -1776,10 +1793,12 @@
       <c r="J26" t="s">
         <v>19</v>
       </c>
-      <c r="K26" s="12"/>
+      <c r="K26" s="12">
+        <v>0.7</v>
+      </c>
       <c r="L26" s="9" t="str">
         <f t="shared" si="0"/>
-        <v>NOK</v>
+        <v>ok</v>
       </c>
       <c r="O26">
         <f t="shared" si="1"/>
@@ -1787,10 +1806,10 @@
       </c>
       <c r="P26">
         <f t="shared" si="2"/>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="27" spans="1:16" x14ac:dyDescent="0.25">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="27" spans="1:16">
       <c r="A27" t="s">
         <v>8</v>
       </c>
@@ -1819,10 +1838,12 @@
       <c r="J27" t="s">
         <v>20</v>
       </c>
-      <c r="K27" s="12"/>
+      <c r="K27" s="12">
+        <v>0.7</v>
+      </c>
       <c r="L27" s="9" t="str">
         <f t="shared" si="0"/>
-        <v>NOK</v>
+        <v>ok</v>
       </c>
       <c r="O27">
         <f t="shared" si="1"/>
@@ -1830,10 +1851,10 @@
       </c>
       <c r="P27">
         <f t="shared" si="2"/>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="28" spans="1:16" x14ac:dyDescent="0.25">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="28" spans="1:16">
       <c r="A28" t="s">
         <v>8</v>
       </c>
@@ -1862,10 +1883,12 @@
       <c r="J28" t="s">
         <v>21</v>
       </c>
-      <c r="K28" s="12"/>
+      <c r="K28" s="12">
+        <v>0.7</v>
+      </c>
       <c r="L28" s="9" t="str">
         <f t="shared" si="0"/>
-        <v>NOK</v>
+        <v>ok</v>
       </c>
       <c r="O28">
         <f t="shared" si="1"/>
@@ -1873,10 +1896,10 @@
       </c>
       <c r="P28">
         <f t="shared" si="2"/>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="29" spans="1:16" x14ac:dyDescent="0.25">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="29" spans="1:16">
       <c r="A29" t="s">
         <v>8</v>
       </c>
@@ -1905,10 +1928,12 @@
       <c r="J29" t="s">
         <v>22</v>
       </c>
-      <c r="K29" s="12"/>
+      <c r="K29" s="12">
+        <v>0.7</v>
+      </c>
       <c r="L29" s="9" t="str">
         <f t="shared" si="0"/>
-        <v>NOK</v>
+        <v>ok</v>
       </c>
       <c r="O29">
         <f t="shared" si="1"/>
@@ -1916,10 +1941,10 @@
       </c>
       <c r="P29">
         <f t="shared" si="2"/>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="30" spans="1:16" x14ac:dyDescent="0.25">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="30" spans="1:16">
       <c r="A30" t="s">
         <v>8</v>
       </c>
@@ -1948,10 +1973,12 @@
       <c r="J30" t="s">
         <v>10</v>
       </c>
-      <c r="K30" s="12"/>
+      <c r="K30" s="12">
+        <v>0.7</v>
+      </c>
       <c r="L30" s="9" t="str">
         <f t="shared" si="0"/>
-        <v>NOK</v>
+        <v>ok</v>
       </c>
       <c r="O30">
         <f t="shared" si="1"/>
@@ -1959,10 +1986,10 @@
       </c>
       <c r="P30">
         <f t="shared" si="2"/>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="31" spans="1:16" x14ac:dyDescent="0.25">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="31" spans="1:16">
       <c r="A31" t="s">
         <v>8</v>
       </c>
@@ -1991,10 +2018,12 @@
       <c r="J31" t="s">
         <v>10</v>
       </c>
-      <c r="K31" s="12"/>
+      <c r="K31" s="12">
+        <v>0.7</v>
+      </c>
       <c r="L31" s="9" t="str">
         <f t="shared" si="0"/>
-        <v>NOK</v>
+        <v>ok</v>
       </c>
       <c r="O31">
         <f t="shared" si="1"/>
@@ -2002,10 +2031,10 @@
       </c>
       <c r="P31">
         <f t="shared" si="2"/>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="32" spans="1:16" x14ac:dyDescent="0.25">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="32" spans="1:16">
       <c r="A32" t="s">
         <v>13</v>
       </c>
@@ -2035,10 +2064,12 @@
       <c r="J32" t="s">
         <v>11</v>
       </c>
-      <c r="K32" s="12"/>
+      <c r="K32" s="12">
+        <v>0.7</v>
+      </c>
       <c r="L32" s="9" t="str">
         <f t="shared" si="0"/>
-        <v>NOK</v>
+        <v>ok</v>
       </c>
       <c r="O32">
         <f t="shared" si="1"/>
@@ -2046,10 +2077,10 @@
       </c>
       <c r="P32">
         <f t="shared" si="2"/>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="33" spans="1:16" x14ac:dyDescent="0.25">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="33" spans="1:16">
       <c r="A33" t="s">
         <v>14</v>
       </c>
@@ -2078,10 +2109,12 @@
       <c r="J33" t="s">
         <v>12</v>
       </c>
-      <c r="K33" s="12"/>
+      <c r="K33" s="12">
+        <v>0.7</v>
+      </c>
       <c r="L33" s="9" t="str">
         <f t="shared" si="0"/>
-        <v>NOK</v>
+        <v>ok</v>
       </c>
       <c r="O33">
         <f t="shared" si="1"/>
@@ -2089,10 +2122,10 @@
       </c>
       <c r="P33">
         <f t="shared" si="2"/>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="34" spans="1:16" x14ac:dyDescent="0.25">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="34" spans="1:16">
       <c r="A34" t="s">
         <v>15</v>
       </c>
@@ -2127,7 +2160,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="35" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:16">
       <c r="A35" t="s">
         <v>16</v>
       </c>
@@ -2157,7 +2190,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="36" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:16">
       <c r="A36" t="s">
         <v>17</v>
       </c>
@@ -2194,7 +2227,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="37" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:16">
       <c r="A37" t="s">
         <v>18</v>
       </c>
@@ -2227,7 +2260,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="38" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:16">
       <c r="A38" t="s">
         <v>19</v>
       </c>
@@ -2256,7 +2289,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="39" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:16">
       <c r="A39" t="s">
         <v>20</v>
       </c>
@@ -2296,7 +2329,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="40" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:16">
       <c r="A40" t="s">
         <v>21</v>
       </c>
@@ -2326,10 +2359,12 @@
       <c r="J40" t="s">
         <v>8</v>
       </c>
-      <c r="K40" s="12"/>
+      <c r="K40" s="12">
+        <v>0.3</v>
+      </c>
       <c r="L40" s="9" t="str">
         <f t="shared" ref="L40:L47" si="5">IF(AND(K40&lt;K$48,ISNUMBER(K40)),"ok","NOK")</f>
-        <v>NOK</v>
+        <v>ok</v>
       </c>
       <c r="O40">
         <f t="shared" si="1"/>
@@ -2337,10 +2372,10 @@
       </c>
       <c r="P40">
         <f t="shared" ref="P40:P47" si="6">IF(L40="NOK",1,0)</f>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="41" spans="1:16" x14ac:dyDescent="0.25">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="41" spans="1:16">
       <c r="A41" t="s">
         <v>26</v>
       </c>
@@ -2370,10 +2405,12 @@
       <c r="J41" t="s">
         <v>8</v>
       </c>
-      <c r="K41" s="12"/>
+      <c r="K41" s="12">
+        <v>0.3</v>
+      </c>
       <c r="L41" s="9" t="str">
         <f t="shared" si="5"/>
-        <v>NOK</v>
+        <v>ok</v>
       </c>
       <c r="O41">
         <f t="shared" si="1"/>
@@ -2381,10 +2418,10 @@
       </c>
       <c r="P41">
         <f t="shared" si="6"/>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="42" spans="1:16" x14ac:dyDescent="0.25">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="42" spans="1:16">
       <c r="A42" t="s">
         <v>28</v>
       </c>
@@ -2414,10 +2451,12 @@
       <c r="J42" t="s">
         <v>9</v>
       </c>
-      <c r="K42" s="12"/>
+      <c r="K42" s="12">
+        <v>0</v>
+      </c>
       <c r="L42" s="9" t="str">
         <f t="shared" si="5"/>
-        <v>NOK</v>
+        <v>ok</v>
       </c>
       <c r="O42">
         <f t="shared" si="1"/>
@@ -2425,10 +2464,10 @@
       </c>
       <c r="P42">
         <f t="shared" si="6"/>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="43" spans="1:16" x14ac:dyDescent="0.25">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="43" spans="1:16">
       <c r="A43" t="s">
         <v>30</v>
       </c>
@@ -2459,10 +2498,12 @@
       <c r="J43" t="s">
         <v>8</v>
       </c>
-      <c r="K43" s="12"/>
+      <c r="K43" s="12">
+        <v>0.3</v>
+      </c>
       <c r="L43" s="9" t="str">
         <f t="shared" si="5"/>
-        <v>NOK</v>
+        <v>ok</v>
       </c>
       <c r="O43">
         <f t="shared" si="1"/>
@@ -2470,10 +2511,10 @@
       </c>
       <c r="P43">
         <f t="shared" si="6"/>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="44" spans="1:16" x14ac:dyDescent="0.25">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="44" spans="1:16">
       <c r="A44" t="s">
         <v>32</v>
       </c>
@@ -2504,10 +2545,12 @@
       <c r="J44" s="11" t="s">
         <v>8</v>
       </c>
-      <c r="K44" s="12"/>
+      <c r="K44" s="12">
+        <v>0.3</v>
+      </c>
       <c r="L44" s="9" t="str">
         <f t="shared" si="5"/>
-        <v>NOK</v>
+        <v>ok</v>
       </c>
       <c r="O44">
         <f t="shared" si="1"/>
@@ -2515,10 +2558,10 @@
       </c>
       <c r="P44">
         <f t="shared" si="6"/>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="45" spans="1:16" x14ac:dyDescent="0.25">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="45" spans="1:16">
       <c r="A45" t="s">
         <v>34</v>
       </c>
@@ -2549,10 +2592,12 @@
       <c r="J45" t="s">
         <v>10</v>
       </c>
-      <c r="K45" s="12"/>
+      <c r="K45" s="12">
+        <v>0</v>
+      </c>
       <c r="L45" s="9" t="str">
         <f t="shared" si="5"/>
-        <v>NOK</v>
+        <v>ok</v>
       </c>
       <c r="O45">
         <f t="shared" si="1"/>
@@ -2560,10 +2605,10 @@
       </c>
       <c r="P45">
         <f t="shared" si="6"/>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="46" spans="1:16" x14ac:dyDescent="0.25">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="46" spans="1:16">
       <c r="A46" t="s">
         <v>12</v>
       </c>
@@ -2593,10 +2638,12 @@
       <c r="J46" s="11" t="s">
         <v>8</v>
       </c>
-      <c r="K46" s="12"/>
+      <c r="K46" s="12">
+        <v>0.3</v>
+      </c>
       <c r="L46" s="9" t="str">
         <f t="shared" si="5"/>
-        <v>NOK</v>
+        <v>ok</v>
       </c>
       <c r="O46">
         <f t="shared" si="1"/>
@@ -2604,10 +2651,10 @@
       </c>
       <c r="P46">
         <f t="shared" si="6"/>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="47" spans="1:16" x14ac:dyDescent="0.25">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="47" spans="1:16">
       <c r="A47" t="s">
         <v>9</v>
       </c>
@@ -2636,10 +2683,12 @@
       <c r="J47" s="11" t="s">
         <v>8</v>
       </c>
-      <c r="K47" s="12"/>
+      <c r="K47" s="12">
+        <v>0.3</v>
+      </c>
       <c r="L47" s="9" t="str">
         <f t="shared" si="5"/>
-        <v>NOK</v>
+        <v>ok</v>
       </c>
       <c r="O47">
         <f t="shared" si="1"/>
@@ -2647,10 +2696,10 @@
       </c>
       <c r="P47">
         <f t="shared" si="6"/>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="48" spans="1:16" x14ac:dyDescent="0.25">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="48" spans="1:16">
       <c r="A48" t="s">
         <v>9</v>
       </c>
@@ -2684,7 +2733,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="49" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:15">
       <c r="A49" t="s">
         <v>10</v>
       </c>
@@ -2712,7 +2761,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="50" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:15">
       <c r="A50" t="s">
         <v>10</v>
       </c>
@@ -2746,7 +2795,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="51" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:15">
       <c r="A51" t="s">
         <v>36</v>
       </c>
@@ -2780,30 +2829,30 @@
         <v>0</v>
       </c>
     </row>
-    <row r="53" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:15">
       <c r="A53" t="s">
         <v>40</v>
       </c>
       <c r="B53" s="14" t="str">
         <f>IF(SUM(O18:O51,P18:P33,P40:P47)&gt;0,"FAIL","PASS")</f>
-        <v>FAIL</v>
-      </c>
-    </row>
-    <row r="55" spans="1:15" ht="18.75" x14ac:dyDescent="0.3">
+        <v>PASS</v>
+      </c>
+    </row>
+    <row r="55" spans="1:15" ht="18.75">
       <c r="A55" s="1" t="s">
         <v>37</v>
       </c>
       <c r="I55" s="1" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="K55" s="5"/>
       <c r="L55" s="5"/>
     </row>
-    <row r="56" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:15">
       <c r="K56" s="5"/>
       <c r="L56" s="5"/>
     </row>
-    <row r="57" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:15">
       <c r="A57" t="s">
         <v>1</v>
       </c>
@@ -2811,15 +2860,15 @@
         <v>38</v>
       </c>
       <c r="I57" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="J57" s="14"/>
       <c r="K57" s="5"/>
       <c r="M57" s="31" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="58" spans="1:15" x14ac:dyDescent="0.25">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="58" spans="1:15">
       <c r="A58" t="s">
         <v>3</v>
       </c>
@@ -2827,36 +2876,38 @@
         <v>43</v>
       </c>
       <c r="I58" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="J58" s="14"/>
       <c r="K58" s="5"/>
       <c r="M58" s="31" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="59" spans="1:15" x14ac:dyDescent="0.25">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="59" spans="1:15">
       <c r="I59" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="J59" s="14"/>
       <c r="K59" s="5"/>
       <c r="M59" s="31" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="60" spans="1:15" x14ac:dyDescent="0.25">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="60" spans="1:15">
       <c r="A60" t="s">
         <v>39</v>
       </c>
-      <c r="B60" s="24"/>
-    </row>
-    <row r="62" spans="1:15" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="B60" s="24" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="62" spans="1:15" ht="18.75">
       <c r="A62" s="1" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="64" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:15">
       <c r="A64" t="s">
         <v>1</v>
       </c>
@@ -2864,10 +2915,10 @@
         <v>42</v>
       </c>
       <c r="I64" t="s">
-        <v>93</v>
-      </c>
-    </row>
-    <row r="65" spans="1:13" x14ac:dyDescent="0.25">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="65" spans="1:13">
       <c r="A65" t="s">
         <v>3</v>
       </c>
@@ -2875,86 +2926,94 @@
         <v>44</v>
       </c>
       <c r="I65" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="J65" s="25"/>
       <c r="K65" s="17"/>
     </row>
-    <row r="66" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:13">
       <c r="B66" t="s">
+        <v>67</v>
+      </c>
+      <c r="I66" t="s">
+        <v>85</v>
+      </c>
+      <c r="K66" s="33">
+        <v>98.8</v>
+      </c>
+      <c r="L66" s="5" t="s">
+        <v>86</v>
+      </c>
+      <c r="M66" s="18" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="67" spans="1:13">
+      <c r="B67" t="s">
         <v>68</v>
       </c>
-      <c r="I66" t="s">
-        <v>86</v>
-      </c>
-      <c r="K66" s="33"/>
-      <c r="L66" s="5" t="s">
-        <v>87</v>
-      </c>
-      <c r="M66" s="18" t="s">
+      <c r="I67" t="s">
         <v>88</v>
       </c>
-    </row>
-    <row r="67" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="B67" t="s">
-        <v>69</v>
-      </c>
-      <c r="I67" t="s">
-        <v>89</v>
-      </c>
-      <c r="K67" s="33"/>
+      <c r="K67" s="33">
+        <v>9.8770000000000007</v>
+      </c>
       <c r="L67" s="5" t="s">
         <v>45</v>
       </c>
       <c r="M67" s="18" t="s">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="68" spans="1:13" x14ac:dyDescent="0.25">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="68" spans="1:13">
       <c r="B68" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="69" spans="1:13" x14ac:dyDescent="0.25">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="69" spans="1:13">
       <c r="I69" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="K69" s="34">
         <f>102000*K67*0.000001</f>
-        <v>0</v>
+        <v>1.0074540000000001</v>
       </c>
       <c r="L69" s="9" t="s">
-        <v>87</v>
-      </c>
-    </row>
-    <row r="70" spans="1:13" x14ac:dyDescent="0.25">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="70" spans="1:13">
       <c r="B70" t="s">
-        <v>71</v>
-      </c>
-      <c r="C70" s="25"/>
+        <v>70</v>
+      </c>
+      <c r="C70" s="25">
+        <v>-1.9199999999999998E-2</v>
+      </c>
       <c r="D70" s="4" t="s">
         <v>45</v>
       </c>
       <c r="I70" s="26" t="s">
-        <v>96</v>
-      </c>
-    </row>
-    <row r="71" spans="1:13" x14ac:dyDescent="0.25">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="71" spans="1:13">
       <c r="B71" t="s">
-        <v>72</v>
-      </c>
-      <c r="C71" s="25"/>
+        <v>71</v>
+      </c>
+      <c r="C71" s="25">
+        <v>1.8100000000000002E-2</v>
+      </c>
       <c r="D71" s="4" t="s">
         <v>45</v>
       </c>
     </row>
-    <row r="72" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:13">
       <c r="B72" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="C72" s="25">
         <f>C71-C70</f>
-        <v>0</v>
+        <v>3.73E-2</v>
       </c>
       <c r="D72" s="4" t="s">
         <v>45</v>
@@ -2969,27 +3028,27 @@
         <v>45</v>
       </c>
       <c r="I72" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="K72" s="19">
         <f>K66+K69</f>
-        <v>0</v>
+        <v>99.807453999999993</v>
       </c>
       <c r="L72" s="9" t="s">
-        <v>87</v>
-      </c>
-    </row>
-    <row r="73" spans="1:13" x14ac:dyDescent="0.25">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="73" spans="1:13">
       <c r="C73" s="25"/>
       <c r="D73" s="17"/>
       <c r="G73" s="26"/>
     </row>
-    <row r="74" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:13">
       <c r="C74" s="25"/>
       <c r="D74" s="4"/>
       <c r="G74" s="26"/>
     </row>
-    <row r="75" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:13">
       <c r="A75" t="s">
         <v>39</v>
       </c>
@@ -2998,10 +3057,10 @@
         <v>FAIL</v>
       </c>
     </row>
-    <row r="77" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:13">
       <c r="B77" s="14"/>
     </row>
-    <row r="78" spans="1:13" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="78" spans="1:13" ht="18.75">
       <c r="A78" s="1" t="s">
         <v>66</v>
       </c>
@@ -3011,15 +3070,19 @@
         <v>REJECTED</v>
       </c>
     </row>
-    <row r="80" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:13">
       <c r="A80" t="s">
         <v>48</v>
       </c>
-      <c r="B80" s="27"/>
+      <c r="B80" s="27" t="s">
+        <v>100</v>
+      </c>
       <c r="E80" s="9" t="s">
         <v>49</v>
       </c>
-      <c r="F80" s="35"/>
+      <c r="F80" s="35">
+        <v>41918</v>
+      </c>
     </row>
   </sheetData>
   <mergeCells count="1">
@@ -3032,7 +3095,6 @@
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.43000000000000005" right="0.43000000000000005" top="0.51181102362204722" bottom="0.43000000000000005" header="0.43000000000000005" footer="0.43000000000000005"/>
-  <pageSetup paperSize="9" scale="61" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
       <mx:PLV Mode="0" OnePage="0" WScale="100"/>

</xml_diff>